<commit_message>
Add calibration and validation information to the North Santiam basin section.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVCALIBandGages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVCALIBandGages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA0A20-008F-4A47-BEB9-7679FA2913D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D659D07-4235-4196-8982-458A48BE9DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
   </bookViews>
   <sheets>
     <sheet name="NSantiam" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
FLOWreports_PEST_SchaferCreek52.xml - Correct the name of the Reach attribute for downstream flow. It was originally Q, but now it is Q_DISCHARG, to distinguish it from Q2WETL, the flow over the banks of the reach into adjacent wetlands. SimulationScenarios_PEST.xml - Uncomment the spinup scenario. Since we added \r1 to the PEST command line that invokes CW3M, we don't need to keep the spinup scenario commented out any more.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVCALIBandGages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVCALIBandGages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D659D07-4235-4196-8982-458A48BE9DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61904A18-3F90-4DFA-8877-28B8D4C9EA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
   </bookViews>
   <sheets>
     <sheet name="NSantiam" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t>Nsantiam HBVCALIB and gages</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t xml:space="preserve"> CLACKAMAS RIVER AT ESTACADA, OR</t>
+  </si>
+  <si>
+    <t>OakGrove40</t>
   </si>
 </sst>
 </file>
@@ -673,56 +676,56 @@
       <selection sqref="A1:R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" customWidth="1"/>
-    <col min="18" max="18" width="33.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="33.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -775,7 +778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>44</v>
       </c>
@@ -834,7 +837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>37</v>
       </c>
@@ -893,7 +896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -949,7 +952,7 @@
         <v>1.0338605160258942</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>0.99298141683982077</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>51</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>1.0120425327329783</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>54</v>
       </c>
@@ -1076,12 +1079,12 @@
       <c r="O15" s="5"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="O16" s="5"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>1.0241558206412413</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1194,23 +1197,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9154E62-0423-4CA0-BDAD-3F7BB1C57B2D}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:Q8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" customWidth="1"/>
     <col min="13" max="17" width="10" customWidth="1"/>
     <col min="27" max="27" width="10" customWidth="1"/>
-    <col min="28" max="28" width="53.109375" customWidth="1"/>
+    <col min="28" max="28" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1218,12 +1221,12 @@
       <c r="G1" s="2"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1231,7 +1234,7 @@
       <c r="G3" s="2"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1239,7 +1242,7 @@
       <c r="G4" s="2"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1247,7 +1250,7 @@
       <c r="G5" s="2"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1331,7 +1334,7 @@
       </c>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>26</v>
       </c>
@@ -1371,7 +1374,7 @@
       </c>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
@@ -1416,14 +1419,49 @@
       <c r="Z8" s="4"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9">
+        <v>23809450</v>
+      </c>
+      <c r="H9">
+        <v>14208700</v>
+      </c>
+      <c r="I9">
+        <v>14143</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9">
+        <v>23810706</v>
+      </c>
+      <c r="N9">
+        <v>54.4</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H11">
-        <v>14208700</v>
+        <v>14209000</v>
       </c>
       <c r="I11">
         <v>14143</v>
@@ -1432,14 +1470,15 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="M11">
-        <v>23810706</v>
+        <v>23809432</v>
       </c>
       <c r="N11">
-        <v>54.4</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="O11" s="10"/>
       <c r="P11" s="9" t="s">
         <v>76</v>
       </c>
@@ -1447,26 +1486,28 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H12">
-        <v>14209000</v>
+        <v>14209250</v>
       </c>
       <c r="I12">
-        <v>14143</v>
+        <v>2555</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <v>273</v>
+      </c>
       <c r="L12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12">
-        <v>23809432</v>
+        <v>79</v>
+      </c>
+      <c r="M12" t="s">
+        <v>80</v>
       </c>
       <c r="N12">
-        <v>124</v>
-      </c>
-      <c r="O12" s="10"/>
+        <v>141</v>
+      </c>
       <c r="P12" s="9" t="s">
         <v>76</v>
       </c>
@@ -1474,58 +1515,29 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H13">
-        <v>14209250</v>
+        <v>14209500</v>
       </c>
       <c r="I13">
-        <v>2555</v>
+        <v>14139</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13">
-        <v>273</v>
-      </c>
       <c r="L13" t="s">
-        <v>79</v>
-      </c>
-      <c r="M13" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="M13">
+        <v>23809158</v>
       </c>
       <c r="N13">
-        <v>141</v>
+        <v>479</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>76</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="H14">
-        <v>14209500</v>
-      </c>
-      <c r="I14">
-        <v>14139</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
-        <v>81</v>
-      </c>
-      <c r="M14">
-        <v>23809158</v>
-      </c>
-      <c r="N14">
-        <v>479</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" s="9" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rough calibration of COT6 in preparation for running PEST. CW3M_WRB.envx - Put the startYear back to 2010. HBV.csv - Change ET_MULT for COT6 from 1.0 to 2.0. FLOWreports_NSantiam.xml - Add a report for Jan Irene Miller's property. IDU_NSantiam.dbf - I'm not sure what changed here. Add PEST_COT6/flow2010.ic. FLOWreports_PEST_COT6.xml - Correct the observation file name. HRU_PEST_COT6.dbf, IDU_PEST_COT6.dbf, Reach_PEST_COT6.dbf - Save spinup results. UNITCONV.H - Correct the FT3_PER_M3 conversion factor! Was 35.29, corrected to 35.3147.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVCALIBandGages.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVCALIBandGages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61904A18-3F90-4DFA-8877-28B8D4C9EA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A95958-8BFF-4E25-9380-C2E2E76FAAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
   </bookViews>
   <sheets>
     <sheet name="NSantiam" sheetId="1" r:id="rId1"/>
@@ -672,60 +672,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED544CC-C2DF-41BC-A13B-027C1D733E2A}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" workbookViewId="0">
-      <selection sqref="A1:R19"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" customWidth="1"/>
-    <col min="18" max="18" width="33.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" customWidth="1"/>
+    <col min="18" max="18" width="33.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -778,7 +779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>44</v>
       </c>
@@ -837,7 +838,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>37</v>
       </c>
@@ -896,7 +897,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -952,7 +953,7 @@
         <v>1.0338605160258942</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>50</v>
       </c>
@@ -1008,7 +1009,7 @@
         <v>0.99298141683982077</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>51</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>1.0120425327329783</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>54</v>
       </c>
@@ -1079,12 +1080,12 @@
       <c r="O15" s="5"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="E16" s="4"/>
       <c r="O16" s="5"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>1.0241558206412413</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1199,21 +1200,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9154E62-0423-4CA0-BDAD-3F7BB1C57B2D}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="37.44140625" customWidth="1"/>
     <col min="13" max="17" width="10" customWidth="1"/>
     <col min="27" max="27" width="10" customWidth="1"/>
-    <col min="28" max="28" width="53.140625" customWidth="1"/>
+    <col min="28" max="28" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1221,12 +1222,12 @@
       <c r="G1" s="2"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1234,7 +1235,7 @@
       <c r="G3" s="2"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1242,7 +1243,7 @@
       <c r="G4" s="2"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1250,7 +1251,7 @@
       <c r="G5" s="2"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1335,7 @@
       </c>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>26</v>
       </c>
@@ -1374,7 +1375,7 @@
       </c>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>28</v>
       </c>
@@ -1419,7 +1420,7 @@
       <c r="Z8" s="4"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>40</v>
       </c>
@@ -1454,12 +1455,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H11">
         <v>14209000</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H12">
         <v>14209250</v>
       </c>
@@ -1515,7 +1516,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="H13">
         <v>14209500</v>
       </c>

</xml_diff>